<commit_message>
user search tc update
</commit_message>
<xml_diff>
--- a/Test Design Specifications/Search_Users_Test_Design_Specifications .xlsx
+++ b/Test Design Specifications/Search_Users_Test_Design_Specifications .xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="102">
   <si>
     <t xml:space="preserve"> Test Design Specification Identifier</t>
   </si>
@@ -330,6 +330,9 @@
   <si>
     <t>no mathch-no results</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -472,11 +475,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -486,18 +495,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:H35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -824,11 +827,11 @@
       <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="32" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="35" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="26"/>
@@ -850,7 +853,7 @@
       <c r="AB1" s="13"/>
     </row>
     <row r="2" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="26"/>
@@ -866,7 +869,7 @@
       <c r="J2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="25"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="26"/>
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
@@ -906,13 +909,13 @@
       <c r="H3" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>65</v>
+      <c r="I3" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>66</v>
       </c>
       <c r="L3" s="26"/>
@@ -934,7 +937,7 @@
       <c r="AB3" s="16"/>
     </row>
     <row r="4" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="26"/>
@@ -946,7 +949,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
-      <c r="K4" s="25"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="26"/>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -986,9 +989,11 @@
       <c r="H5" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J5" s="12"/>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="28" t="s">
         <v>81</v>
       </c>
       <c r="L5" s="26"/>
@@ -1034,8 +1039,8 @@
         <v>82</v>
       </c>
       <c r="J6" s="12"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
@@ -1078,7 +1083,7 @@
         <v>82</v>
       </c>
       <c r="J7" s="12"/>
-      <c r="K7" s="27"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="26"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
@@ -1122,7 +1127,7 @@
         <v>82</v>
       </c>
       <c r="J8" s="12"/>
-      <c r="K8" s="25"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="26"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
@@ -1166,7 +1171,7 @@
         <v>82</v>
       </c>
       <c r="J9" s="12"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="26"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
@@ -1206,9 +1211,11 @@
       <c r="H10" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J10" s="12"/>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="28" t="s">
         <v>84</v>
       </c>
       <c r="L10" s="26"/>
@@ -1254,10 +1261,10 @@
       <c r="J11" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="L11" s="29"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="22" t="s">
         <v>99</v>
       </c>
@@ -1304,10 +1311,10 @@
       <c r="J12" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L12" s="29"/>
+      <c r="L12" s="31"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
@@ -1348,10 +1355,10 @@
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="L13" s="29"/>
+      <c r="L13" s="31"/>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -1392,10 +1399,10 @@
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="20"/>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="29"/>
+      <c r="L14" s="31"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
@@ -1436,8 +1443,8 @@
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
@@ -1478,10 +1485,10 @@
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="L16" s="29"/>
+      <c r="L16" s="31"/>
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
@@ -1524,10 +1531,10 @@
       <c r="J17" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="29"/>
+      <c r="L17" s="31"/>
       <c r="M17" s="24"/>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -1570,10 +1577,10 @@
       <c r="J18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="30"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
@@ -1616,10 +1623,10 @@
       <c r="J19" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L19" s="30"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
@@ -1662,10 +1669,10 @@
       <c r="J20" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="30"/>
+      <c r="L20" s="32"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
@@ -1710,10 +1717,10 @@
       <c r="J21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L21" s="29"/>
+      <c r="L21" s="31"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
@@ -1758,10 +1765,10 @@
       <c r="J22" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="30"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
@@ -1780,7 +1787,7 @@
       <c r="AB22" s="24"/>
     </row>
     <row r="23" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="26"/>
@@ -1792,7 +1799,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
-      <c r="K23" s="25"/>
+      <c r="K23" s="27"/>
       <c r="L23" s="26"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -1836,7 +1843,7 @@
         <v>82</v>
       </c>
       <c r="J24" s="12"/>
-      <c r="K24" s="25"/>
+      <c r="K24" s="27"/>
       <c r="L24" s="26"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -1882,7 +1889,7 @@
       <c r="J25" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="28" t="s">
         <v>67</v>
       </c>
       <c r="L25" s="26"/>
@@ -2105,7 +2112,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="31"/>
+      <c r="H32" s="29"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="16"/>
@@ -2135,7 +2142,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
-      <c r="H33" s="31"/>
+      <c r="H33" s="29"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="16"/>
@@ -2165,7 +2172,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="31"/>
+      <c r="H34" s="29"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="16"/>
@@ -2195,7 +2202,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="31"/>
+      <c r="H35" s="29"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="16"/>
@@ -31589,28 +31596,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="H32:H35"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
@@ -31619,6 +31604,28 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="H32:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -31671,11 +31678,11 @@
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="32" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="35" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="26"/>
@@ -31697,7 +31704,7 @@
       <c r="AB1" s="2"/>
     </row>
     <row r="2" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="26"/>
@@ -31713,7 +31720,7 @@
       <c r="J2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="25"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="26"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -31759,7 +31766,7 @@
       <c r="J3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>66</v>
       </c>
       <c r="L3" s="26"/>
@@ -31781,7 +31788,7 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="26"/>
@@ -31793,7 +31800,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="25"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="26"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -31837,7 +31844,7 @@
         <v>91</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="28" t="s">
         <v>81</v>
       </c>
       <c r="L5" s="26"/>
@@ -31883,8 +31890,8 @@
         <v>82</v>
       </c>
       <c r="J6" s="7"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -31927,7 +31934,7 @@
         <v>82</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="27"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="26"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -31971,7 +31978,7 @@
         <v>82</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="25"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="26"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -32015,7 +32022,7 @@
         <v>82</v>
       </c>
       <c r="J9" s="7"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="26"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -32059,7 +32066,7 @@
         <v>65</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="28" t="s">
         <v>84</v>
       </c>
       <c r="L10" s="26"/>
@@ -32107,10 +32114,10 @@
       <c r="J11" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="L11" s="29"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="19" t="s">
         <v>99</v>
       </c>
@@ -32159,10 +32166,10 @@
       <c r="J12" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L12" s="29"/>
+      <c r="L12" s="31"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -32205,10 +32212,10 @@
         <v>65</v>
       </c>
       <c r="J13" s="20"/>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="L13" s="29"/>
+      <c r="L13" s="31"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -32251,10 +32258,10 @@
         <v>65</v>
       </c>
       <c r="J14" s="20"/>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="29"/>
+      <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
@@ -32297,8 +32304,8 @@
         <v>65</v>
       </c>
       <c r="J15" s="20"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -32341,10 +32348,10 @@
         <v>65</v>
       </c>
       <c r="J16" s="20"/>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="L16" s="29"/>
+      <c r="L16" s="31"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -32389,10 +32396,10 @@
       <c r="J17" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="29"/>
+      <c r="L17" s="31"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -32437,10 +32444,10 @@
       <c r="J18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="30"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -32485,10 +32492,10 @@
       <c r="J19" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L19" s="30"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -32533,10 +32540,10 @@
       <c r="J20" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="30"/>
+      <c r="L20" s="32"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -32581,10 +32588,10 @@
       <c r="J21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L21" s="29"/>
+      <c r="L21" s="31"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -32629,10 +32636,10 @@
       <c r="J22" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="30"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -32651,7 +32658,7 @@
       <c r="AB22" s="18"/>
     </row>
     <row r="23" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="26"/>
@@ -32663,7 +32670,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="25"/>
+      <c r="K23" s="27"/>
       <c r="L23" s="26"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -32707,7 +32714,7 @@
         <v>82</v>
       </c>
       <c r="J24" s="7"/>
-      <c r="K24" s="25"/>
+      <c r="K24" s="27"/>
       <c r="L24" s="26"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -32753,7 +32760,7 @@
       <c r="J25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="28" t="s">
         <v>67</v>
       </c>
       <c r="L25" s="26"/>
@@ -32976,7 +32983,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="31"/>
+      <c r="H32" s="29"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="3"/>
@@ -33006,7 +33013,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="31"/>
+      <c r="H33" s="29"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="3"/>
@@ -33036,7 +33043,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="31"/>
+      <c r="H34" s="29"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="3"/>
@@ -33066,7 +33073,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="31"/>
+      <c r="H35" s="29"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="3"/>
@@ -62460,6 +62467,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="H32:H35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="I1:J1"/>
@@ -62476,20 +62497,6 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="A23:G23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>